<commit_message>
Moved User to SharedClasses, Working on errors on DAL
</commit_message>
<xml_diff>
--- a/DAL/UsersDB.xlsx
+++ b/DAL/UsersDB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guyal\Desktop\SecurityTK\DAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rOTEM\Documents\SecurityTK\DAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -135,11 +135,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -148,21 +148,21 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -215,8 +215,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="היפר-קישור" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -260,7 +260,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -525,16 +525,16 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="17.625" customWidth="1"/>
-    <col min="2" max="2" width="14.375" customWidth="1"/>
+    <col min="1" max="1" width="17.6328125" customWidth="1"/>
+    <col min="2" max="2" width="14.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -542,7 +542,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -550,7 +550,7 @@
         <v>12345678</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -558,7 +558,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -566,7 +566,7 @@
         <v>12341234</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -574,7 +574,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -582,7 +582,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -590,7 +590,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -598,7 +598,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -606,7 +606,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -614,7 +614,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -622,7 +622,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -630,7 +630,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -638,7 +638,7 @@
         <v>11111111</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -646,7 +646,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -654,7 +654,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -662,7 +662,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -670,7 +670,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -678,7 +678,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -686,7 +686,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -694,7 +694,7 @@
         <v>12121212</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed all problems. The code is working.
</commit_message>
<xml_diff>
--- a/DAL/UsersDB.xlsx
+++ b/DAL/UsersDB.xlsx
@@ -110,9 +110,6 @@
     <t>monkey12</t>
   </si>
   <si>
-    <t>letmein1</t>
-  </si>
-  <si>
     <t>access22</t>
   </si>
   <si>
@@ -129,6 +126,9 @@
   </si>
   <si>
     <t>mustang1</t>
+  </si>
+  <si>
+    <t>dm8k26h2</t>
   </si>
 </sst>
 </file>
@@ -619,7 +619,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -643,7 +643,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -651,7 +651,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -659,7 +659,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -667,7 +667,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -675,7 +675,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -683,7 +683,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:2">

</xml_diff>